<commit_message>
starting to read excel with python ;
</commit_message>
<xml_diff>
--- a/shots/players/senor_wetball.xlsx
+++ b/shots/players/senor_wetball.xlsx
@@ -19,12 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Senor</t>
   </si>
   <si>
     <t>Wetball</t>
+  </si>
+  <si>
+    <t>hi</t>
   </si>
 </sst>
 </file>
@@ -394,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>10</v>
       </c>
@@ -418,7 +421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>15</v>
       </c>
@@ -426,12 +429,143 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>27</v>
       </c>
       <c r="B4">
         <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <f>B4-3</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B11" si="0">B5-3</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <f>A6+1</f>
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <f t="shared" ref="A8:A17" si="1">A7+1</f>
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <f>B11+2</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:B17" si="2">B12+2</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>